<commit_message>
new demande creation matricule sifac
</commit_message>
<xml_diff>
--- a/upload/demande_de_creation_de_matricule_sifac.xlsx
+++ b/upload/demande_de_creation_de_matricule_sifac.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaina Tighilt\Desktop\AMU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaina.tighilt\Nextcloud\AMU_portable\Bureau\AMU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFD03529-F9DE-433F-8BEB-2E25E612D885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{77CE80B8-E45C-4963-A9D0-83ADA091EBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3DE8090D-E3DB-478E-8442-4B8300185FB0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3DE8090D-E3DB-478E-8442-4B8300185FB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1929,7 +1929,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>1562100</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>31750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1996,7 +1996,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>1562100</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>31750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2055,15 +2055,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>85725</xdr:colOff>
+          <xdr:colOff>88900</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>800100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>1076325</xdr:colOff>
+          <xdr:colOff>1079500</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>488950</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2112,7 +2112,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2141,13 +2141,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:colOff>565150</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>14</xdr:col>
-          <xdr:colOff>47625</xdr:colOff>
+          <xdr:colOff>50800</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
@@ -2198,7 +2198,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2229,7 +2229,7 @@
           <xdr:col>7</xdr:col>
           <xdr:colOff>1162050</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>146050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
@@ -2284,7 +2284,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2313,15 +2313,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>504825</xdr:colOff>
+          <xdr:colOff>508000</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>371475</xdr:colOff>
+          <xdr:colOff>374650</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>752475</xdr:rowOff>
+          <xdr:rowOff>755650</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2370,7 +2370,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2399,15 +2399,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>600075</xdr:colOff>
+          <xdr:colOff>603250</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>180975</xdr:rowOff>
+          <xdr:rowOff>184150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>523875</xdr:colOff>
+          <xdr:colOff>527050</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>771525</xdr:rowOff>
+          <xdr:rowOff>774700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2456,7 +2456,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2485,13 +2485,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1022350</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>1343025</xdr:colOff>
+          <xdr:colOff>1346200</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>762000</xdr:rowOff>
         </xdr:to>
@@ -2542,7 +2542,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2571,13 +2571,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1022350</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>15</xdr:col>
-          <xdr:colOff>523875</xdr:colOff>
+          <xdr:colOff>527050</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>800100</xdr:rowOff>
         </xdr:to>
@@ -2628,7 +2628,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2657,13 +2657,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:colOff>565150</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1038225</xdr:colOff>
+          <xdr:colOff>1041400</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
@@ -2726,11 +2726,11 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>533400</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>1133475</xdr:colOff>
+          <xdr:colOff>1136650</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>95250</xdr:rowOff>
         </xdr:to>
@@ -2793,13 +2793,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>165100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>990600</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>428625</xdr:rowOff>
+          <xdr:rowOff>431800</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2848,7 +2848,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2879,13 +2879,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>542925</xdr:rowOff>
+          <xdr:rowOff>546100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>1485900</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>809625</xdr:rowOff>
+          <xdr:rowOff>812800</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2934,7 +2934,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2963,15 +2963,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>66675</xdr:colOff>
+          <xdr:colOff>69850</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>942975</xdr:rowOff>
+          <xdr:rowOff>946150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>371475</xdr:colOff>
+          <xdr:colOff>374650</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>1171575</xdr:rowOff>
+          <xdr:rowOff>1174750</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3020,7 +3020,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3110,13 +3110,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:colOff>565150</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>1038225</xdr:colOff>
+          <xdr:colOff>1041400</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
@@ -3481,26 +3481,26 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" customWidth="1"/>
+    <col min="6" max="6" width="23.1796875" customWidth="1"/>
+    <col min="7" max="7" width="26.81640625" customWidth="1"/>
+    <col min="8" max="8" width="29.81640625" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="22.5703125" customWidth="1"/>
-    <col min="12" max="12" width="22.28515625" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" customWidth="1"/>
+    <col min="11" max="11" width="22.54296875" customWidth="1"/>
+    <col min="12" max="12" width="22.26953125" customWidth="1"/>
+    <col min="14" max="14" width="25.1796875" customWidth="1"/>
+    <col min="15" max="15" width="13.54296875" customWidth="1"/>
+    <col min="16" max="16" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B8" s="47"/>
       <c r="C8" s="48"/>
       <c r="D8" s="48"/>
@@ -3519,7 +3519,7 @@
       <c r="O8" s="48"/>
       <c r="P8" s="57"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B9" s="44"/>
       <c r="C9" s="45"/>
       <c r="D9" s="45"/>
@@ -3538,7 +3538,7 @@
       <c r="O9" s="45"/>
       <c r="P9" s="57"/>
     </row>
-    <row r="10" spans="2:17" s="1" customFormat="1" ht="105.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" s="1" customFormat="1" ht="105.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="39" t="s">
         <v>21</v>
       </c>
@@ -3563,7 +3563,7 @@
       <c r="O10" s="43"/>
       <c r="P10" s="72"/>
     </row>
-    <row r="11" spans="2:17" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>0</v>
       </c>
@@ -3575,7 +3575,7 @@
       <c r="I11" s="51"/>
       <c r="P11" s="52"/>
     </row>
-    <row r="12" spans="2:17" s="1" customFormat="1" ht="48.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" s="1" customFormat="1" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="5" t="s">
         <v>2</v>
       </c>
@@ -3596,7 +3596,7 @@
       <c r="O12" s="73"/>
       <c r="P12" s="74"/>
     </row>
-    <row r="13" spans="2:17" s="1" customFormat="1" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" s="1" customFormat="1" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="8" t="s">
         <v>29</v>
       </c>
@@ -3613,7 +3613,7 @@
       <c r="K13" s="9"/>
       <c r="P13" s="52"/>
     </row>
-    <row r="14" spans="2:17" s="1" customFormat="1" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:17" s="1" customFormat="1" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="98" t="s">
         <v>7</v>
       </c>
@@ -3639,7 +3639,7 @@
       <c r="P14" s="76"/>
       <c r="Q14" s="71"/>
     </row>
-    <row r="15" spans="2:17" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="102"/>
       <c r="C15" s="103"/>
       <c r="D15" s="103"/>
@@ -3656,7 +3656,7 @@
       <c r="O15" s="22"/>
       <c r="P15" s="58"/>
     </row>
-    <row r="16" spans="2:17" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="13" t="s">
         <v>12</v>
       </c>
@@ -3681,7 +3681,7 @@
       <c r="O16" s="56"/>
       <c r="P16" s="38"/>
     </row>
-    <row r="17" spans="2:16" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" ht="44.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="100" t="s">
         <v>15</v>
       </c>
@@ -3706,7 +3706,7 @@
       <c r="O17" s="109"/>
       <c r="P17" s="110"/>
     </row>
-    <row r="18" spans="2:16" s="1" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:16" s="1" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="13" t="s">
         <v>8</v>
       </c>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="P18" s="17"/>
     </row>
-    <row r="19" spans="2:16" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="89" t="s">
         <v>27</v>
       </c>
@@ -3760,7 +3760,7 @@
       <c r="O19" s="83"/>
       <c r="P19" s="84"/>
     </row>
-    <row r="20" spans="2:16" ht="95.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" ht="95.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="92"/>
       <c r="C20" s="93"/>
       <c r="D20" s="93"/>
@@ -3777,7 +3777,7 @@
       <c r="O20" s="86"/>
       <c r="P20" s="87"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B21" s="92"/>
       <c r="C21" s="93"/>
       <c r="D21" s="93"/>
@@ -3794,7 +3794,7 @@
       <c r="O21" s="86"/>
       <c r="P21" s="87"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B22" s="92"/>
       <c r="C22" s="93"/>
       <c r="D22" s="93"/>
@@ -3811,7 +3811,7 @@
       <c r="O22" s="86"/>
       <c r="P22" s="87"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B23" s="92"/>
       <c r="C23" s="93"/>
       <c r="D23" s="93"/>
@@ -3828,7 +3828,7 @@
       <c r="O23" s="61"/>
       <c r="P23" s="62"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B24" s="92"/>
       <c r="C24" s="93"/>
       <c r="D24" s="93"/>
@@ -3851,7 +3851,7 @@
       <c r="O24" s="107"/>
       <c r="P24" s="108"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B25" s="92"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
@@ -3868,7 +3868,7 @@
       <c r="O25" s="107"/>
       <c r="P25" s="108"/>
     </row>
-    <row r="26" spans="2:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="95"/>
       <c r="C26" s="96"/>
       <c r="D26" s="96"/>
@@ -3927,7 +3927,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>1562100</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>31750</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3949,7 +3949,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>1562100</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>31750</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3963,15 +3963,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>85725</xdr:colOff>
+                    <xdr:colOff>88900</xdr:colOff>
                     <xdr:row>13</xdr:row>
                     <xdr:rowOff>800100</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>1076325</xdr:colOff>
+                    <xdr:colOff>1079500</xdr:colOff>
                     <xdr:row>14</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>488950</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3985,13 +3985,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:colOff>565150</xdr:colOff>
                     <xdr:row>14</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>14</xdr:col>
-                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:colOff>50800</xdr:colOff>
                     <xdr:row>15</xdr:row>
                     <xdr:rowOff>76200</xdr:rowOff>
                   </to>
@@ -4009,7 +4009,7 @@
                     <xdr:col>7</xdr:col>
                     <xdr:colOff>1162050</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>146050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>8</xdr:col>
@@ -4029,15 +4029,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>504825</xdr:colOff>
+                    <xdr:colOff>508000</xdr:colOff>
                     <xdr:row>15</xdr:row>
                     <xdr:rowOff>190500</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>371475</xdr:colOff>
+                    <xdr:colOff>374650</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>752475</xdr:rowOff>
+                    <xdr:rowOff>755650</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4051,15 +4051,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>600075</xdr:colOff>
+                    <xdr:colOff>603250</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>180975</xdr:rowOff>
+                    <xdr:rowOff>184150</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>523875</xdr:colOff>
+                    <xdr:colOff>527050</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>771525</xdr:rowOff>
+                    <xdr:rowOff>774700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4073,13 +4073,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>10</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1022350</xdr:colOff>
                     <xdr:row>15</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>11</xdr:col>
-                    <xdr:colOff>1343025</xdr:colOff>
+                    <xdr:colOff>1346200</xdr:colOff>
                     <xdr:row>15</xdr:row>
                     <xdr:rowOff>762000</xdr:rowOff>
                   </to>
@@ -4095,13 +4095,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>11</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1022350</xdr:colOff>
                     <xdr:row>15</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>15</xdr:col>
-                    <xdr:colOff>523875</xdr:colOff>
+                    <xdr:colOff>527050</xdr:colOff>
                     <xdr:row>15</xdr:row>
                     <xdr:rowOff>800100</xdr:rowOff>
                   </to>
@@ -4117,13 +4117,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:colOff>565150</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1038225</xdr:colOff>
+                    <xdr:colOff>1041400</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>76200</xdr:rowOff>
                   </to>
@@ -4141,11 +4141,11 @@
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>533400</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>1133475</xdr:colOff>
+                    <xdr:colOff>1136650</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>95250</xdr:rowOff>
                   </to>
@@ -4163,13 +4163,13 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>165100</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>990600</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>428625</xdr:rowOff>
+                    <xdr:rowOff>431800</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4185,13 +4185,13 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>542925</xdr:rowOff>
+                    <xdr:rowOff>546100</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>1485900</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>809625</xdr:rowOff>
+                    <xdr:rowOff>812800</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4205,15 +4205,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>66675</xdr:colOff>
+                    <xdr:colOff>69850</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>942975</xdr:rowOff>
+                    <xdr:rowOff>946150</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>371475</xdr:colOff>
+                    <xdr:colOff>374650</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>1171575</xdr:rowOff>
+                    <xdr:rowOff>1174750</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4227,13 +4227,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>561975</xdr:colOff>
+                    <xdr:colOff>565150</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>1038225</xdr:colOff>
+                    <xdr:colOff>1041400</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>76200</xdr:rowOff>
                   </to>

</xml_diff>